<commit_message>
Fixed a bug in Lookup API (Build 465)
</commit_message>
<xml_diff>
--- a/doc/Planning/Features-Status.xlsx
+++ b/doc/Planning/Features-Status.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\babaksoft\Projects\SPPC\framework\doc\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eslamieh\Projects\framework\doc\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -471,6 +471,558 @@
   </cellStyles>
   <dxfs count="42">
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <strike val="0"/>
@@ -491,558 +1043,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="medium">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="medium">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="medium">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1113,55 +1113,55 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D41" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <autoFilter ref="A2:D41"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="امکان پایه" dataDxfId="0"/>
-    <tableColumn id="2" name="شرح قابلیت" dataDxfId="1"/>
-    <tableColumn id="3" name="توضیحات" dataDxfId="36"/>
-    <tableColumn id="7" name="موارد باقی‌مانده" dataDxfId="35"/>
+    <tableColumn id="1" name="امکان پایه" dataDxfId="36"/>
+    <tableColumn id="2" name="شرح قابلیت" dataDxfId="35"/>
+    <tableColumn id="3" name="توضیحات" dataDxfId="34"/>
+    <tableColumn id="7" name="موارد باقی‌مانده" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:F17" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:F17" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="A2:F17"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="هدف کاری" dataDxfId="29"/>
-    <tableColumn id="2" name="قابلیت" dataDxfId="28"/>
-    <tableColumn id="5" name="اولویت" dataDxfId="27"/>
-    <tableColumn id="6" name="مسئول انجام" dataDxfId="26"/>
-    <tableColumn id="3" name="وضعیت انجام" dataDxfId="25"/>
-    <tableColumn id="7" name="توضیحات" dataDxfId="24"/>
+    <tableColumn id="1" name="هدف کاری" dataDxfId="27"/>
+    <tableColumn id="2" name="قابلیت" dataDxfId="26"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="25"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="24"/>
+    <tableColumn id="3" name="وضعیت انجام" dataDxfId="23"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table146" displayName="Table146" ref="A2:F17" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table146" displayName="Table146" ref="A2:F17" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="A2:F17"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="هدف کاری" dataDxfId="18"/>
-    <tableColumn id="2" name="قابلیت" dataDxfId="17"/>
-    <tableColumn id="5" name="اولویت" dataDxfId="16"/>
-    <tableColumn id="6" name="مسئول انجام" dataDxfId="15"/>
-    <tableColumn id="3" name="وضعیت انجام" dataDxfId="14"/>
-    <tableColumn id="7" name="توضیحات" dataDxfId="13"/>
+    <tableColumn id="1" name="هدف کاری" dataDxfId="16"/>
+    <tableColumn id="2" name="قابلیت" dataDxfId="15"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="14"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="13"/>
+    <tableColumn id="3" name="وضعیت انجام" dataDxfId="12"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1465" displayName="Table1465" ref="A2:F17" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1465" displayName="Table1465" ref="A2:F17" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A2:F17"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="هدف کاری" dataDxfId="7"/>
-    <tableColumn id="2" name="قابلیت" dataDxfId="6"/>
-    <tableColumn id="5" name="اولویت" dataDxfId="5"/>
-    <tableColumn id="6" name="مسئول انجام" dataDxfId="4"/>
-    <tableColumn id="3" name="وضعیت انجام" dataDxfId="3"/>
-    <tableColumn id="7" name="توضیحات" dataDxfId="2"/>
+    <tableColumn id="1" name="هدف کاری" dataDxfId="5"/>
+    <tableColumn id="2" name="قابلیت" dataDxfId="4"/>
+    <tableColumn id="5" name="اولویت" dataDxfId="3"/>
+    <tableColumn id="6" name="مسئول انجام" dataDxfId="2"/>
+    <tableColumn id="3" name="وضعیت انجام" dataDxfId="1"/>
+    <tableColumn id="7" name="توضیحات" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1432,24 +1432,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" customWidth="1"/>
-    <col min="3" max="3" width="49.21875" customWidth="1"/>
-    <col min="4" max="4" width="78.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="78.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="118.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="3" t="s">
         <v>16</v>
@@ -1487,7 +1487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
@@ -1497,7 +1497,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="3" t="s">
         <v>21</v>
@@ -1507,7 +1507,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="3" t="s">
         <v>23</v>
@@ -1517,7 +1517,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="3" t="s">
         <v>28</v>
@@ -1539,7 +1539,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>30</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="193.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="193.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>33</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="133.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="133.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="3" t="s">
         <v>36</v>
@@ -1575,7 +1575,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>39</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="3" t="s">
         <v>42</v>
@@ -1597,7 +1597,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="3" t="s">
         <v>43</v>
@@ -1605,7 +1605,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
         <v>44</v>
@@ -1613,7 +1613,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="3" t="s">
         <v>45</v>
@@ -1621,7 +1621,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>54</v>
       </c>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="3" t="s">
         <v>48</v>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="3" t="s">
         <v>49</v>
@@ -1651,7 +1651,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="3" t="s">
         <v>50</v>
@@ -1659,7 +1659,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="3" t="s">
         <v>51</v>
@@ -1667,7 +1667,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="3" t="s">
         <v>64</v>
@@ -1675,7 +1675,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>55</v>
       </c>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="3" t="s">
         <v>57</v>
@@ -1695,7 +1695,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="3" t="s">
         <v>58</v>
@@ -1703,7 +1703,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>59</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="3" t="s">
         <v>61</v>
@@ -1723,7 +1723,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="3" t="s">
         <v>62</v>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="3" t="s">
         <v>65</v>
@@ -1741,7 +1741,7 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>67</v>
       </c>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="3" t="s">
         <v>69</v>
@@ -1761,7 +1761,7 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>71</v>
       </c>
@@ -1771,7 +1771,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="3" t="s">
         <v>73</v>
@@ -1779,7 +1779,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="3" t="s">
         <v>77</v>
@@ -1791,7 +1791,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="3" t="s">
         <v>76</v>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="3" t="s">
         <v>79</v>
@@ -1813,7 +1813,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>82</v>
       </c>
@@ -1825,19 +1825,19 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1860,22 +1860,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.109375" customWidth="1"/>
-    <col min="2" max="2" width="57.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.5546875" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -1903,7 +1903,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -1911,7 +1911,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -1919,7 +1919,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -1927,7 +1927,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -1935,7 +1935,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -1943,7 +1943,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
@@ -1951,7 +1951,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -1959,7 +1959,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
@@ -1967,7 +1967,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -1975,7 +1975,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -1983,7 +1983,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -1991,7 +1991,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -1999,7 +1999,7 @@
       <c r="E15" s="8"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -2007,7 +2007,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -2015,70 +2015,70 @@
       <c r="E17" s="8"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E39" s="5"/>
     </row>
   </sheetData>
@@ -2106,22 +2106,22 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.109375" customWidth="1"/>
-    <col min="2" max="2" width="58.44140625" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.88671875" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -2149,7 +2149,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -2157,7 +2157,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -2165,7 +2165,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -2173,7 +2173,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -2181,7 +2181,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -2189,7 +2189,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
@@ -2197,7 +2197,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -2205,7 +2205,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
@@ -2213,7 +2213,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -2221,7 +2221,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -2229,7 +2229,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -2237,7 +2237,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -2245,7 +2245,7 @@
       <c r="E15" s="8"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -2253,7 +2253,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -2261,70 +2261,70 @@
       <c r="E17" s="8"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E39" s="5"/>
     </row>
   </sheetData>
@@ -2351,22 +2351,22 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.109375" customWidth="1"/>
-    <col min="2" max="2" width="58.44140625" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.88671875" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -2394,7 +2394,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -2402,7 +2402,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -2410,7 +2410,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -2418,7 +2418,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -2426,7 +2426,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -2434,7 +2434,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
@@ -2442,7 +2442,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -2450,7 +2450,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
@@ -2458,7 +2458,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
@@ -2466,7 +2466,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -2474,7 +2474,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
@@ -2482,7 +2482,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -2490,7 +2490,7 @@
       <c r="E15" s="8"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -2498,7 +2498,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -2506,70 +2506,70 @@
       <c r="E17" s="8"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E39" s="5"/>
     </row>
   </sheetData>

</xml_diff>